<commit_message>
falta diagrama de gantt
Mañana a primera hora descargo la aplicacion par lo del diagrama
</commit_message>
<xml_diff>
--- a/Documentación/cuadro comparativo.xlsx
+++ b/Documentación/cuadro comparativo.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juan_\OneDrive\Escritorio\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{81EE16F7-FC0F-4B9D-B330-365193DD64C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{0F37CDCF-5C71-493D-BAA6-619A1969E848}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -137,10 +131,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="170" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -209,14 +203,11 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -233,7 +224,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -248,14 +239,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -318,7 +312,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -370,7 +364,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -564,223 +558,223 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C16CE53-172C-45C6-9BE9-A205A2870C62}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.42578125" customWidth="1"/>
-    <col min="2" max="2" width="49.7109375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="49.7109375" style="5" customWidth="1"/>
     <col min="3" max="3" width="37.42578125" customWidth="1"/>
     <col min="4" max="4" width="22.28515625" customWidth="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="8">
         <v>2999900</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="16">
+      <c r="E4" s="15">
         <v>2499900</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="16">
+      <c r="E5" s="15">
         <v>1791000</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="16">
+      <c r="E6" s="15">
         <v>1359900</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="240" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="14">
+      <c r="E7" s="13">
         <v>1387500</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="4" t="s">
+      <c r="A11" s="2"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="71.25" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="8">
         <v>3900</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="8">
         <v>8900</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="8">
         <v>12900</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="128.25" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="8">
         <v>8200</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13" s="8">
         <v>15200</v>
       </c>
-      <c r="E13" s="9">
+      <c r="E13" s="8">
         <v>24400</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="71.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C14" s="8">
         <v>0</v>
       </c>
-      <c r="D14" s="9">
+      <c r="D14" s="8">
         <v>96254</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E14" s="8">
         <v>962543</v>
       </c>
     </row>
@@ -912,12 +906,13 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" display="https://www.falabella.com.co/falabella-co/search?Ntt=&amp;f.product.brandName=Huawei" xr:uid="{D1BDC83A-2AD5-4AEF-9F1D-3A116C421051}"/>
-    <hyperlink ref="A4" r:id="rId2" display="https://www.falabella.com.co/falabella-co/search?Ntt=&amp;f.product.brandName=HP" xr:uid="{15FF9A73-80BB-4FB2-AF78-01531A824C03}"/>
-    <hyperlink ref="A5" r:id="rId3" display="https://www.falabella.com.co/falabella-co/search?Ntt=&amp;f.product.brandName=JANUS" xr:uid="{8B1C6CB0-1B0D-4C60-834B-7C3FE5086BB8}"/>
-    <hyperlink ref="A6" r:id="rId4" display="https://www.falabella.com.co/falabella-co/search?Ntt=&amp;f.product.brandName=Asus" xr:uid="{8F164AB5-CBB9-4DA1-88A7-B98DC60E41FE}"/>
-    <hyperlink ref="A7" r:id="rId5" display="https://www.falabella.com.co/falabella-co/search?Ntt=&amp;f.product.brandName=Lenovo" xr:uid="{6C2BA4FA-378D-49C3-9B2B-BD1B3CD6F820}"/>
+    <hyperlink ref="A3" r:id="rId1" display="https://www.falabella.com.co/falabella-co/search?Ntt=&amp;f.product.brandName=Huawei"/>
+    <hyperlink ref="A4" r:id="rId2" display="https://www.falabella.com.co/falabella-co/search?Ntt=&amp;f.product.brandName=HP"/>
+    <hyperlink ref="A5" r:id="rId3" display="https://www.falabella.com.co/falabella-co/search?Ntt=&amp;f.product.brandName=JANUS"/>
+    <hyperlink ref="A6" r:id="rId4" display="https://www.falabella.com.co/falabella-co/search?Ntt=&amp;f.product.brandName=Asus"/>
+    <hyperlink ref="A7" r:id="rId5" display="https://www.falabella.com.co/falabella-co/search?Ntt=&amp;f.product.brandName=Lenovo"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>